<commit_message>
Finalize before Maarten's fault handling changes
Was never tested, but should have worked prior to Maarten's fault
handling changes and CAN rewrite
</commit_message>
<xml_diff>
--- a/PulseSync/Notes.xlsx
+++ b/PulseSync/Notes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -16,20 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>Actions to make the pulse sync board work for the 2.5MeV system</t>
   </si>
   <si>
-    <t>Since there are no status fibers from PFN, Gun or RF, the PIC will need to send status to clear these "faults"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Either need to lift the outputs of the schmidt triggers (U48-2, U48-8, and U48-6) </t>
-  </si>
-  <si>
-    <t>Or remove U49-2 and put 5V on the pin.</t>
-  </si>
-  <si>
     <t>Must install jumpers on W1 and W2 for keylock and panel switch status to PIC</t>
   </si>
   <si>
@@ -70,6 +61,21 @@
   </si>
   <si>
     <t>Pulse Sync Board</t>
+  </si>
+  <si>
+    <t>CAN Communication jumpers</t>
+  </si>
+  <si>
+    <t>Cut trace on W6, W7, W9 (solder side)</t>
+  </si>
+  <si>
+    <t>Install jumpers in W4, W8, W10</t>
+  </si>
+  <si>
+    <t>Since there are no status fibers from PFN or Gun, the PIC will need to send status to clear these "faults"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Either need to lift the outputs of the schmidt triggers (U48-2, U48-8) </t>
   </si>
 </sst>
 </file>
@@ -415,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -439,35 +445,48 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
-        <v>3</v>
+      <c r="B5" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="C6" t="s">
         <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
-        <v>6</v>
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -479,7 +498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -492,30 +511,30 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="L1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2">
         <v>10000000</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I3">
         <v>29100000</v>
       </c>
       <c r="L3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="M3" s="2">
         <v>32768</v>
@@ -523,21 +542,21 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B4" s="4">
         <f>B3/B5/10</f>
         <v>15625</v>
       </c>
       <c r="H4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I4">
         <f>I3/256/10</f>
         <v>11367.1875</v>
       </c>
       <c r="L4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="M4">
         <f>HEX2DEC(8000)</f>
@@ -546,22 +565,22 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>64</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I5">
         <v>256</v>
       </c>
       <c r="L5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="M5">
         <v>1</v>
@@ -569,24 +588,24 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2">
         <f>1/B3</f>
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I7">
         <f>1/I3</f>
         <v>3.4364261168384879E-8</v>
       </c>
       <c r="L7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="M7" s="2">
         <f>1/M3</f>
@@ -595,24 +614,24 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3">
         <f>B7*B5*B4</f>
         <v>9.9999999999999992E-2</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="I8">
         <f>I7*I5*I4</f>
         <v>9.9999999999999992E-2</v>
       </c>
       <c r="L8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="M8" s="2">
         <f>M7*M5*M4</f>

</xml_diff>